<commit_message>
Changes in Action Suite files for Gowri Task Action Entity completion such as added few files: ActionCreation, ActionUpdate,ActionWorkflow etc, change name of existing files and change in Test Suite base and xls files
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Action Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Action Suite.xlsx
@@ -4,21 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="ActionCreation" sheetId="3" r:id="rId2"/>
-    <sheet name="InterpretationCreation" sheetId="4" r:id="rId3"/>
-    <sheet name="IssueCreation" sheetId="5" r:id="rId4"/>
-    <sheet name="ChangeRequestCreation" sheetId="6" r:id="rId5"/>
+    <sheet name="ActionWorkflow" sheetId="7" r:id="rId2"/>
+    <sheet name="ActionUpdate" sheetId="8" r:id="rId3"/>
+    <sheet name="ActionCreation" sheetId="3" r:id="rId4"/>
+    <sheet name="InterpretationCreation" sheetId="4" r:id="rId5"/>
+    <sheet name="IssueCreation" sheetId="5" r:id="rId6"/>
+    <sheet name="ChangeRequestCreation" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="135">
   <si>
     <t>TCID</t>
   </si>
@@ -227,24 +229,9 @@
     <t>actionSupplierAccess</t>
   </si>
   <si>
-    <t>actionRequestedOnMonth</t>
-  </si>
-  <si>
     <t>actionRequestedOnDate</t>
   </si>
   <si>
-    <t>actionRequestedOnYear</t>
-  </si>
-  <si>
-    <t>actionDueDateMonth</t>
-  </si>
-  <si>
-    <t>actionDueDateDate</t>
-  </si>
-  <si>
-    <t>actionDueDateYear</t>
-  </si>
-  <si>
     <t>actionFinancialImpact</t>
   </si>
   <si>
@@ -350,21 +337,6 @@
     <t>ActionWorkflow</t>
   </si>
   <si>
-    <t>ActionWorkflow description</t>
-  </si>
-  <si>
-    <t>action from ip1</t>
-  </si>
-  <si>
-    <t>ac desc</t>
-  </si>
-  <si>
-    <t>Action Type 101 Edit Again</t>
-  </si>
-  <si>
-    <t>Tier1 Edit</t>
-  </si>
-  <si>
     <t>Interpretation</t>
   </si>
   <si>
@@ -392,7 +364,67 @@
     <t>cr from ac1</t>
   </si>
   <si>
+    <t>actionDueDate</t>
+  </si>
+  <si>
+    <t>Root Cause Analysis</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Asia/Kathmandu (GMT +05:45)</t>
+  </si>
+  <si>
+    <t>Tier - 1</t>
+  </si>
+  <si>
+    <t>Joint Action</t>
+  </si>
+  <si>
+    <t>Joint Actions are initiated to implement the Strategic Research and Innovation Agenda </t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>December-12-2016</t>
+  </si>
+  <si>
+    <t>February-2-2018</t>
+  </si>
+  <si>
+    <t>actionTaken</t>
+  </si>
+  <si>
+    <t>Corrective and preventive action</t>
+  </si>
+  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>ActionUpdate</t>
+  </si>
+  <si>
+    <t>Compensatory damages</t>
+  </si>
+  <si>
+    <t>Pay money to reimburse costs and compensate for losses</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>America/Caracas (GMT -04:30)</t>
+  </si>
+  <si>
+    <t>January-13-2017</t>
+  </si>
+  <si>
+    <t>March-13-2017</t>
   </si>
 </sst>
 </file>
@@ -400,7 +432,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,8 +447,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF434343"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +496,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -514,6 +566,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="justify"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,17 +916,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -885,11 +951,9 @@
         <v>63</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -900,11 +964,9 @@
         <v>65</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,27 +977,40 @@
         <v>67</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -944,10 +1019,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="5" max="16384" style="17" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="3" max="4" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="20">
+        <v>100</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="20"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,18 +1198,19 @@
     <col min="2" max="2" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="21.140625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="22.28515625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="9" max="11" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="15.5703125" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="13" max="15" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="16" max="19" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="14" max="15" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1008,88 +1251,64 @@
         <v>69</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="M2" s="9">
-        <v>2</v>
-      </c>
-      <c r="N2" s="9">
-        <v>21</v>
-      </c>
-      <c r="O2" s="9">
-        <v>2011</v>
-      </c>
-      <c r="P2" s="9">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="9">
-        <v>5</v>
-      </c>
-      <c r="R2" s="9">
-        <v>2017</v>
-      </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="Q2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="2"/>
+      <c r="R2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1097,7 +1316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -1125,61 +1344,61 @@
     <col min="16" max="16" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
     <col min="18" max="18" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>2</v>
@@ -1193,16 +1412,16 @@
     </row>
     <row r="2" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>15</v>
@@ -1252,7 +1471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -1283,7 +1502,7 @@
     <col min="19" max="19" bestFit="true" customWidth="true" width="32.28515625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
     <col min="21" max="21" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -1315,13 +1534,13 @@
         <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>31</v>
@@ -1330,22 +1549,22 @@
         <v>30</v>
       </c>
       <c r="O1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>29</v>
@@ -1362,13 +1581,13 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>15</v>
@@ -1429,11 +1648,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
@@ -1457,7 +1676,7 @@
     <col min="23" max="23" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
     <col min="25" max="25" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -1481,7 +1700,7 @@
         <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>54</v>
@@ -1499,22 +1718,22 @@
         <v>50</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>49</v>
@@ -1546,17 +1765,17 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>15</v>

</xml_diff>